<commit_message>
looking for a cointegrated panel
</commit_message>
<xml_diff>
--- a/test-results/Cointegration/Cointegration_results_2.xlsx
+++ b/test-results/Cointegration/Cointegration_results_2.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caw6/Desktop/UrbanizationCauseConsequence/test-results/Cointegration/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16900" windowHeight="17620"/>
   </bookViews>
@@ -16,20 +11,12 @@
     <sheet name="PctPopUrbanGDPRealUSD" sheetId="2" r:id="rId2"/>
     <sheet name="GDPPerCapRealUSDPctPopUrban" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0" fullCalcOnLoad="true" concurrentCalc="false"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="162">
   <si>
     <t>Country</t>
   </si>
@@ -520,8 +507,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -616,11 +603,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -886,19 +868,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P147"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="true" showRuler="false" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="12" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="16" width="12.6640625" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -948,7 +930,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -992,13 +974,13 @@
         <v>-16.251422159071002</v>
       </c>
       <c r="O2">
-        <v>-18.040670518023258</v>
+        <v>-2.5638043529732282</v>
       </c>
       <c r="P2">
         <v>-17.725416525748539</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -1042,13 +1024,13 @@
         <v>-11.75523230782334</v>
       </c>
       <c r="O3">
-        <v>-12.124795192440899</v>
+        <v>-1.9333293013201871</v>
       </c>
       <c r="P3">
         <v>-12.411272998751789</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" t="s">
         <v>99</v>
       </c>
@@ -1092,13 +1074,13 @@
         <v>-16.74458260556078</v>
       </c>
       <c r="O4">
-        <v>-16.128387224167788</v>
+        <v>-2.5015872292678432</v>
       </c>
       <c r="P4">
         <v>-15.683414516712309</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -1142,13 +1124,13 @@
         <v>-6.0024154595864676</v>
       </c>
       <c r="O5">
-        <v>-5.6232983257116684</v>
+        <v>-2.595009255364269</v>
       </c>
       <c r="P5">
         <v>-4.9990936510257926</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" t="s">
         <v>120</v>
       </c>
@@ -1192,13 +1174,13 @@
         <v>-6.161073546908681</v>
       </c>
       <c r="O6">
-        <v>-6.0613666365157206</v>
+        <v>-2.7904622454973569</v>
       </c>
       <c r="P6">
         <v>-5.9977700718950508</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1242,13 +1224,13 @@
         <v>-6.7342332926050306</v>
       </c>
       <c r="O7">
-        <v>-7.2453164054770776</v>
+        <v>-2.2128553639228921</v>
       </c>
       <c r="P7">
         <v>-8.1088775866599825</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" t="s">
         <v>136</v>
       </c>
@@ -1292,13 +1274,13 @@
         <v>-4.864249273367161</v>
       </c>
       <c r="O8">
-        <v>-4.8164369576977446</v>
+        <v>-1.727101771729634</v>
       </c>
       <c r="P8">
         <v>-4.4619440215830179</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -1342,13 +1324,13 @@
         <v>-5.0553968505092328</v>
       </c>
       <c r="O9">
-        <v>-5.8972549820172491</v>
+        <v>1.1896713589043659</v>
       </c>
       <c r="P9">
         <v>-6.995216083019141</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1392,13 +1374,13 @@
         <v>-3.4296961536604278</v>
       </c>
       <c r="O10">
-        <v>-3.324317226211376</v>
+        <v>-2.0599921269573329</v>
       </c>
       <c r="P10">
         <v>-3.2973581164053338</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1442,13 +1424,13 @@
         <v>-5.2926907720478527</v>
       </c>
       <c r="O11">
-        <v>-5.2703563903582751</v>
+        <v>-0.58885984623404464</v>
       </c>
       <c r="P11">
         <v>-6.1188249935627308</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -1492,13 +1474,13 @@
         <v>-3.637414268747087</v>
       </c>
       <c r="O12">
-        <v>-3.9450832163289009</v>
+        <v>-2.4849063860753509</v>
       </c>
       <c r="P12">
         <v>-4.0264868614104001</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -1542,13 +1524,13 @@
         <v>-3.9247978672070309</v>
       </c>
       <c r="O13">
-        <v>-3.514929380728069</v>
+        <v>-1.528034942999013</v>
       </c>
       <c r="P13">
         <v>-3.7287712323027198</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -1592,13 +1574,13 @@
         <v>-2.6509742953915039</v>
       </c>
       <c r="O14">
-        <v>-2.416895584734418</v>
+        <v>-0.58521144759678034</v>
       </c>
       <c r="P14">
         <v>-2.2304072694886892</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -1642,13 +1624,13 @@
         <v>-2.10291741888051</v>
       </c>
       <c r="O15">
-        <v>-1.881905889801972</v>
+        <v>-2.4146984047149802</v>
       </c>
       <c r="P15">
         <v>-1.626905533135331</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1692,13 +1674,13 @@
         <v>-2.1124602252714881</v>
       </c>
       <c r="O16">
-        <v>-1.9333293013201871</v>
+        <v>-1.0794431210827149</v>
       </c>
       <c r="P16">
         <v>-1.445403535867601</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -1742,13 +1724,13 @@
         <v>-2.3979684378089079</v>
       </c>
       <c r="O17">
-        <v>-2.2471789866673308</v>
+        <v>-0.79047591821232599</v>
       </c>
       <c r="P17">
         <v>-2.0995899775237721</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" t="s">
         <v>144</v>
       </c>
@@ -1792,13 +1774,13 @@
         <v>-2.427705907016275</v>
       </c>
       <c r="O18">
-        <v>-2.2091532010369912</v>
+        <v>-0.69620251389204446</v>
       </c>
       <c r="P18">
         <v>-2.195443586331117</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" t="s">
         <v>142</v>
       </c>
@@ -1842,13 +1824,13 @@
         <v>-3.3179511571319602</v>
       </c>
       <c r="O19">
-        <v>-3.538723149636597</v>
+        <v>-1.4387138410440981</v>
       </c>
       <c r="P19">
         <v>-3.705216386228058</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -1892,13 +1874,13 @@
         <v>-1.949773501228838</v>
       </c>
       <c r="O20">
-        <v>-1.8835200148229341</v>
+        <v>-2.0814111831035502</v>
       </c>
       <c r="P20">
         <v>-1.7640639347838021</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -1942,13 +1924,13 @@
         <v>-2.659998484576465</v>
       </c>
       <c r="O21">
-        <v>-2.7585320079900182</v>
+        <v>-2.17876494731996</v>
       </c>
       <c r="P21">
         <v>-2.0954656012608242</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1992,13 +1974,13 @@
         <v>-3.1706200008492158</v>
       </c>
       <c r="O22">
-        <v>-3.1675980229825562</v>
+        <v>-2.222137521538802</v>
       </c>
       <c r="P22">
         <v>-3.0759975335161158</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -2042,13 +2024,13 @@
         <v>-3.1855081912057708</v>
       </c>
       <c r="O23">
-        <v>-3.5531123571160199</v>
+        <v>-1.498301796825479</v>
       </c>
       <c r="P23">
         <v>-4.0505731240140808</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -2092,13 +2074,13 @@
         <v>-3.0568518594001448</v>
       </c>
       <c r="O24">
-        <v>-3.1139172834254851</v>
+        <v>-2.0602729846840679</v>
       </c>
       <c r="P24">
         <v>-2.722387554386609</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -2142,13 +2124,13 @@
         <v>-3.0519011348277321</v>
       </c>
       <c r="O25">
-        <v>-3.4765063281912112</v>
+        <v>-5.2703563903582751</v>
       </c>
       <c r="P25">
         <v>-3.6648674928775642</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -2192,13 +2174,13 @@
         <v>-2.881388508194251</v>
       </c>
       <c r="O26">
-        <v>-3.173196083845732</v>
+        <v>-1.951162019417475</v>
       </c>
       <c r="P26">
         <v>-3.051545482000678</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" t="s">
         <v>124</v>
       </c>
@@ -2242,13 +2224,13 @@
         <v>-2.573676582247244</v>
       </c>
       <c r="O27">
-        <v>-2.1948338957660471</v>
+        <v>-3.324317226211376</v>
       </c>
       <c r="P27">
         <v>-2.1419182069703209</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -2292,13 +2274,13 @@
         <v>-3.2320809907344841</v>
       </c>
       <c r="O28">
-        <v>-2.595009255364269</v>
+        <v>-2.1063300609021458</v>
       </c>
       <c r="P28">
         <v>-2.7378626870395699</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -2342,13 +2324,13 @@
         <v>-2.348771004184425</v>
       </c>
       <c r="O29">
-        <v>-2.150949543969837</v>
+        <v>-2.071912764624495</v>
       </c>
       <c r="P29">
         <v>-2.1699851652743232</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -2392,13 +2374,13 @@
         <v>-2.1271023586706992</v>
       </c>
       <c r="O30">
-        <v>-1.8192268771293709</v>
+        <v>-1.1084819198036899</v>
       </c>
       <c r="P30">
         <v>-1.930012028708604</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -2442,13 +2424,13 @@
         <v>-2.7281060795292782</v>
       </c>
       <c r="O31">
-        <v>-2.4146984047149802</v>
+        <v>-1.308767918691963</v>
       </c>
       <c r="P31">
         <v>-1.8499950550923061</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" t="s">
         <v>98</v>
       </c>
@@ -2492,13 +2474,13 @@
         <v>-3.1805686683391632</v>
       </c>
       <c r="O32">
-        <v>-3.006878062117893</v>
+        <v>-1.8192268771293709</v>
       </c>
       <c r="P32">
         <v>-3.2589781362522299</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -2542,13 +2524,13 @@
         <v>-2.5947801612857062</v>
       </c>
       <c r="O33">
-        <v>-2.222137521538802</v>
+        <v>-3.1675980229825562</v>
       </c>
       <c r="P33">
         <v>-1.1660280074607521</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34">
       <c r="A34" t="s">
         <v>121</v>
       </c>
@@ -2592,13 +2574,13 @@
         <v>-2.2318584630363101</v>
       </c>
       <c r="O34">
-        <v>-2.1994665822257979</v>
+        <v>-1.378615170960996</v>
       </c>
       <c r="P34">
         <v>-2.198325554132964</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -2642,13 +2624,13 @@
         <v>-2.1765643657820668</v>
       </c>
       <c r="O35">
-        <v>-2.17876494731996</v>
+        <v>-2.1197420544188161</v>
       </c>
       <c r="P35">
         <v>-2.2579860161069569</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36">
       <c r="A36" t="s">
         <v>91</v>
       </c>
@@ -2692,13 +2674,13 @@
         <v>-2.2220182544898832</v>
       </c>
       <c r="O36">
-        <v>-1.9340209619469131</v>
+        <v>-0.59645923001078116</v>
       </c>
       <c r="P36">
         <v>-1.966560713004857</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37">
       <c r="A37" t="s">
         <v>27</v>
       </c>
@@ -2742,13 +2724,13 @@
         <v>-2.6288428968428592</v>
       </c>
       <c r="O37">
-        <v>-2.1063300609021458</v>
+        <v>-1.968824181252067</v>
       </c>
       <c r="P37">
         <v>-2.35765974895966</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -2792,13 +2774,13 @@
         <v>-2.9860106482717739</v>
       </c>
       <c r="O38">
-        <v>-2.748641818731179</v>
+        <v>-2.0573093779077372</v>
       </c>
       <c r="P38">
         <v>-2.495437632118517</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -2842,13 +2824,13 @@
         <v>-2.1334803710827668</v>
       </c>
       <c r="O39">
-        <v>-2.0573093779077372</v>
+        <v>-0.99079914278383074</v>
       </c>
       <c r="P39">
         <v>-2.0539770627198002</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -2892,13 +2874,13 @@
         <v>-2.5981088853298679</v>
       </c>
       <c r="O40">
-        <v>-2.5015872292678432</v>
+        <v>-7.2453164054770776</v>
       </c>
       <c r="P40">
         <v>-2.2333620943866932</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41">
       <c r="A41" t="s">
         <v>102</v>
       </c>
@@ -2942,13 +2924,13 @@
         <v>-2.0500985392281992</v>
       </c>
       <c r="O41">
-        <v>-1.602659131324522</v>
+        <v>-2.166306004480218</v>
       </c>
       <c r="P41">
         <v>-1.133496167387114</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42">
       <c r="A42" t="s">
         <v>113</v>
       </c>
@@ -2992,13 +2974,13 @@
         <v>-2.4029011970525112</v>
       </c>
       <c r="O42">
-        <v>-2.6341214830080371</v>
+        <v>-1.923017801874819</v>
       </c>
       <c r="P42">
         <v>-1.774178809397617</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43">
       <c r="A43" t="s">
         <v>62</v>
       </c>
@@ -3042,13 +3024,13 @@
         <v>-2.4746467441460518</v>
       </c>
       <c r="O43">
-        <v>-2.8000208103686219</v>
+        <v>-2.1908010983117299</v>
       </c>
       <c r="P43">
         <v>-2.827684712859035</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -3092,13 +3074,13 @@
         <v>-1.811685136192555</v>
       </c>
       <c r="O44">
-        <v>-1.708218596908089</v>
+        <v>-2.748641818731179</v>
       </c>
       <c r="P44">
         <v>-1.7710342231483489</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45">
       <c r="A45" t="s">
         <v>25</v>
       </c>
@@ -3142,13 +3124,13 @@
         <v>-2.0729594808709062</v>
       </c>
       <c r="O45">
-        <v>-1.951162019417475</v>
+        <v>-2.4506051342417101</v>
       </c>
       <c r="P45">
         <v>-1.967628372577652</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -3192,13 +3174,13 @@
         <v>-2.5499285347455491</v>
       </c>
       <c r="O46">
-        <v>-2.4506051342417101</v>
+        <v>-18.040670518023258</v>
       </c>
       <c r="P46">
         <v>-2.0865415009458621</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -3242,13 +3224,13 @@
         <v>-2.1862567048540811</v>
       </c>
       <c r="O47">
-        <v>-1.968824181252067</v>
+        <v>-2.1213339977736392</v>
       </c>
       <c r="P47">
         <v>-2.0023036468898052</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48">
       <c r="A48" t="s">
         <v>139</v>
       </c>
@@ -3292,13 +3274,13 @@
         <v>-2.7623580718540151</v>
       </c>
       <c r="O48">
-        <v>-2.5160300971999372</v>
+        <v>-1.557857847788215</v>
       </c>
       <c r="P48">
         <v>-2.5031576739548251</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49">
       <c r="A49" t="s">
         <v>87</v>
       </c>
@@ -3342,13 +3324,13 @@
         <v>-2.25405869024581</v>
       </c>
       <c r="O49">
-        <v>-2.5101645918006712</v>
+        <v>-1.708218596908089</v>
       </c>
       <c r="P49">
         <v>-2.0617406420036648</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50">
       <c r="A50" t="s">
         <v>34</v>
       </c>
@@ -3392,13 +3374,13 @@
         <v>-2.175453910237271</v>
       </c>
       <c r="O50">
-        <v>-2.1197420544188161</v>
+        <v>-0.81815043665245191</v>
       </c>
       <c r="P50">
         <v>-1.968849876602998</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -3442,13 +3424,13 @@
         <v>-1.6941090534197989</v>
       </c>
       <c r="O51">
-        <v>-1.727101771729634</v>
+        <v>-3.4765063281912112</v>
       </c>
       <c r="P51">
         <v>-1.7153103118674771</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52">
       <c r="A52" t="s">
         <v>33</v>
       </c>
@@ -3492,13 +3474,13 @@
         <v>-1.847675064369247</v>
       </c>
       <c r="O52">
-        <v>-1.378615170960996</v>
+        <v>-2.000421963789123</v>
       </c>
       <c r="P52">
         <v>-1.432529249514918</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -3542,13 +3524,13 @@
         <v>-2.1141217883363428</v>
       </c>
       <c r="O53">
-        <v>-2.2128553639228921</v>
+        <v>-0.83575044073620497</v>
       </c>
       <c r="P53">
         <v>-2.2613577736523149</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54">
       <c r="A54" t="s">
         <v>100</v>
       </c>
@@ -3592,13 +3574,13 @@
         <v>-2.105575175236079</v>
       </c>
       <c r="O54">
-        <v>-2.234557968804844</v>
+        <v>-1.882344554530639</v>
       </c>
       <c r="P54">
         <v>-2.4102532613525889</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55">
       <c r="A55" t="s">
         <v>127</v>
       </c>
@@ -3642,13 +3624,13 @@
         <v>-1.1257089458346741</v>
       </c>
       <c r="O55">
-        <v>-1.1303461262420711</v>
+        <v>-0.57679142768196268</v>
       </c>
       <c r="P55">
         <v>-1.208817888807538</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56">
       <c r="A56" t="s">
         <v>105</v>
       </c>
@@ -3692,13 +3674,13 @@
         <v>-2.5723825236212829</v>
       </c>
       <c r="O56">
-        <v>-3.1557623644588721</v>
+        <v>-3.173196083845732</v>
       </c>
       <c r="P56">
         <v>-3.591280357811891</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -3742,13 +3724,13 @@
         <v>-1.482905269530171</v>
       </c>
       <c r="O57">
-        <v>-1.4387138410440981</v>
+        <v>-0.86795587885461012</v>
       </c>
       <c r="P57">
         <v>-1.277631430173366</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58">
       <c r="A58" t="s">
         <v>73</v>
       </c>
@@ -3792,13 +3774,13 @@
         <v>-2.0688880931520881</v>
       </c>
       <c r="O58">
-        <v>-2.0347814564705229</v>
+        <v>-2.416895584734418</v>
       </c>
       <c r="P58">
         <v>-2.0956737001704902</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -3842,13 +3824,13 @@
         <v>-2.1297966071161669</v>
       </c>
       <c r="O59">
-        <v>-2.3039521631149542</v>
+        <v>-1.552935003874216</v>
       </c>
       <c r="P59">
         <v>-2.093258234165114</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60">
       <c r="A60" t="s">
         <v>130</v>
       </c>
@@ -3892,13 +3874,13 @@
         <v>-2.195577429343754</v>
       </c>
       <c r="O60">
-        <v>-2.1690494492313031</v>
+        <v>-0.31960062222834362</v>
       </c>
       <c r="P60">
         <v>-1.962036768003063</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61">
       <c r="A61" t="s">
         <v>129</v>
       </c>
@@ -3942,13 +3924,13 @@
         <v>-2.139397419565209</v>
       </c>
       <c r="O61">
-        <v>-2.1514519230217051</v>
+        <v>-2.3039521631149542</v>
       </c>
       <c r="P61">
         <v>-2.0707367532998999</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -3992,13 +3974,13 @@
         <v>-2.3533014387273532</v>
       </c>
       <c r="O62">
-        <v>-2.4849063860753509</v>
+        <v>-1.884701478940177</v>
       </c>
       <c r="P62">
         <v>-2.3736550734817099</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63">
       <c r="A63" t="s">
         <v>86</v>
       </c>
@@ -4042,13 +4024,13 @@
         <v>-1.3144016084819929</v>
       </c>
       <c r="O63">
-        <v>-1.219490598262444</v>
+        <v>-2.8000208103686219</v>
       </c>
       <c r="P63">
         <v>-1.0151190982505089</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="64">
       <c r="A64" t="s">
         <v>40</v>
       </c>
@@ -4092,13 +4074,13 @@
         <v>-2.1970552624143602</v>
       </c>
       <c r="O64">
-        <v>-2.166306004480218</v>
+        <v>-0.46892191352523233</v>
       </c>
       <c r="P64">
         <v>-2.0715768034177811</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65">
       <c r="A65" t="s">
         <v>47</v>
       </c>
@@ -4142,13 +4124,13 @@
         <v>-1.3802252944447699</v>
       </c>
       <c r="O65">
-        <v>-1.557857847788215</v>
+        <v>-1.5292953896156209</v>
       </c>
       <c r="P65">
         <v>-1.454091936488582</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="66">
       <c r="A66" t="s">
         <v>116</v>
       </c>
@@ -4192,13 +4174,13 @@
         <v>-2.1143628088482318</v>
       </c>
       <c r="O66">
-        <v>-2.619289920597569</v>
+        <v>-2.4766821776990469</v>
       </c>
       <c r="P66">
         <v>-1.9354910103352101</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="67">
       <c r="A67" t="s">
         <v>5</v>
       </c>
@@ -4242,13 +4224,13 @@
         <v>-2.3689298192185899</v>
       </c>
       <c r="O67">
-        <v>-2.7904622454973569</v>
+        <v>-1.4166974892347779</v>
       </c>
       <c r="P67">
         <v>-2.426046323792991</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="68">
       <c r="A68" t="s">
         <v>71</v>
       </c>
@@ -4292,13 +4274,13 @@
         <v>-2.3075271068599119</v>
       </c>
       <c r="O68">
-        <v>-2.5527275254083501</v>
+        <v>-3.276025622554219</v>
       </c>
       <c r="P68">
         <v>-2.2146873932079472</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="69">
       <c r="A69" t="s">
         <v>115</v>
       </c>
@@ -4342,13 +4324,13 @@
         <v>-2.3576934649791861</v>
       </c>
       <c r="O69">
-        <v>-2.2776806176397701</v>
+        <v>-2.150949543969837</v>
       </c>
       <c r="P69">
         <v>-2.0564709406084472</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="70">
       <c r="A70" t="s">
         <v>84</v>
       </c>
@@ -4392,13 +4374,13 @@
         <v>-1.7537591108238451</v>
       </c>
       <c r="O70">
-        <v>-1.922956133221897</v>
+        <v>0.2279088621277465</v>
       </c>
       <c r="P70">
         <v>-1.6413115912647449</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="71">
       <c r="A71" t="s">
         <v>46</v>
       </c>
@@ -4442,13 +4424,13 @@
         <v>-1.964353769781614</v>
       </c>
       <c r="O71">
-        <v>-2.1213339977736392</v>
+        <v>-1.8835200148229341</v>
       </c>
       <c r="P71">
         <v>-1.890654399358388</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="72">
       <c r="A72" t="s">
         <v>92</v>
       </c>
@@ -4492,13 +4474,13 @@
         <v>-1.7351248234758121</v>
       </c>
       <c r="O72">
-        <v>-1.896026509636713</v>
+        <v>-2.5527275254083501</v>
       </c>
       <c r="P72">
         <v>-1.6977193973348641</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="73">
       <c r="A73" t="s">
         <v>134</v>
       </c>
@@ -4542,13 +4524,13 @@
         <v>-1.876394684170801</v>
       </c>
       <c r="O73">
-        <v>-2.4996639170257571</v>
+        <v>-3.1139172834254851</v>
       </c>
       <c r="P73">
         <v>-2.3352360954668678</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="74">
       <c r="A74" t="s">
         <v>132</v>
       </c>
@@ -4592,13 +4574,13 @@
         <v>-2.0102192807183328</v>
       </c>
       <c r="O74">
-        <v>-1.881898909100997</v>
+        <v>-2.0347814564705229</v>
       </c>
       <c r="P74">
         <v>-1.6391935849430079</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="75">
       <c r="A75" t="s">
         <v>23</v>
       </c>
@@ -4642,13 +4624,13 @@
         <v>-2.1135382987666511</v>
       </c>
       <c r="O75">
-        <v>-2.0602729846840679</v>
+        <v>-1.344125740527178</v>
       </c>
       <c r="P75">
         <v>-1.863814403450812</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="76">
       <c r="A76" t="s">
         <v>94</v>
       </c>
@@ -4692,13 +4674,13 @@
         <v>-2.2821382860463659</v>
       </c>
       <c r="O76">
-        <v>-2.1518223022991601</v>
+        <v>-3.5531123571160199</v>
       </c>
       <c r="P76">
         <v>-2.32204155592484</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="77">
       <c r="A77" t="s">
         <v>114</v>
       </c>
@@ -4742,13 +4724,13 @@
         <v>-2.009107614476195</v>
       </c>
       <c r="O77">
-        <v>-2.112233498473584</v>
+        <v>-1.258331271851314</v>
       </c>
       <c r="P77">
         <v>-2.3023192629655171</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="78">
       <c r="A78" t="s">
         <v>59</v>
       </c>
@@ -4792,13 +4774,13 @@
         <v>-1.0625014518790949</v>
       </c>
       <c r="O78">
-        <v>-0.31960062222834362</v>
+        <v>-3.3039302312256331</v>
       </c>
       <c r="P78">
         <v>0.35830221624369912</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="79">
       <c r="A79" t="s">
         <v>65</v>
       </c>
@@ -4842,13 +4824,13 @@
         <v>-1.8421782039948511</v>
       </c>
       <c r="O79">
-        <v>-2.4766821776990469</v>
+        <v>-1.9961549048662059</v>
       </c>
       <c r="P79">
         <v>-3.1233451662396199</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="80">
       <c r="A80" t="s">
         <v>19</v>
       </c>
@@ -4892,13 +4874,13 @@
         <v>-1.658577336965755</v>
       </c>
       <c r="O80">
-        <v>-2.0814111831035502</v>
+        <v>-2.3457625400034261</v>
       </c>
       <c r="P80">
         <v>-2.4245999787383492</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="81">
       <c r="A81" t="s">
         <v>42</v>
       </c>
@@ -4942,13 +4924,13 @@
         <v>-2.092334055052131</v>
       </c>
       <c r="O81">
-        <v>-2.1908010983117299</v>
+        <v>-5.6232983257116684</v>
       </c>
       <c r="P81">
         <v>-2.154418892848188</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="82">
       <c r="A82" t="s">
         <v>77</v>
       </c>
@@ -4992,13 +4974,13 @@
         <v>-3.425587483993338</v>
       </c>
       <c r="O82">
-        <v>-3.3039302312256331</v>
+        <v>-2.3046135189108452</v>
       </c>
       <c r="P82">
         <v>-2.5403087068366759</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="83">
       <c r="A83" t="s">
         <v>103</v>
       </c>
@@ -5042,13 +5024,13 @@
         <v>-3.2162220303239368</v>
       </c>
       <c r="O83">
-        <v>-2.807380829680707</v>
+        <v>-1.178253605740319</v>
       </c>
       <c r="P83">
         <v>-3.6621198673636139</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="84">
       <c r="A84" t="s">
         <v>106</v>
       </c>
@@ -5092,13 +5074,13 @@
         <v>-1.7651667561988851</v>
       </c>
       <c r="O84">
-        <v>-2.131620143027297</v>
+        <v>-2.2471789866673308</v>
       </c>
       <c r="P84">
         <v>-2.3572667653289008</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="85">
       <c r="A85" t="s">
         <v>81</v>
       </c>
@@ -5142,13 +5124,13 @@
         <v>-2.516196452806835</v>
       </c>
       <c r="O85">
-        <v>-2.3046135189108452</v>
+        <v>-1.922956133221897</v>
       </c>
       <c r="P85">
         <v>-2.068214467727608</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="86">
       <c r="A86" t="s">
         <v>28</v>
       </c>
@@ -5192,13 +5174,13 @@
         <v>-1.5943393464007101</v>
       </c>
       <c r="O86">
-        <v>-2.071912764624495</v>
+        <v>-1.4982244064000521</v>
       </c>
       <c r="P86">
         <v>-1.827058198595815</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="87">
       <c r="A87" t="s">
         <v>74</v>
       </c>
@@ -5242,13 +5224,13 @@
         <v>-1.360754460098673</v>
       </c>
       <c r="O87">
-        <v>-1.344125740527178</v>
+        <v>-1.219490598262444</v>
       </c>
       <c r="P87">
         <v>-1.2769907146113419</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="88">
       <c r="A88" t="s">
         <v>12</v>
       </c>
@@ -5292,13 +5274,13 @@
         <v>-1.4665317252449479</v>
       </c>
       <c r="O88">
-        <v>-1.528034942999013</v>
+        <v>-2.5101645918006712</v>
       </c>
       <c r="P88">
         <v>-1.730883147675764</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="89">
       <c r="A89" t="s">
         <v>90</v>
       </c>
@@ -5342,13 +5324,13 @@
         <v>-2.2037592060136801</v>
       </c>
       <c r="O89">
-        <v>-2.2991768927130232</v>
+        <v>-3.514929380728069</v>
       </c>
       <c r="P89">
         <v>-2.1276580292906559</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="90">
       <c r="A90" t="s">
         <v>141</v>
       </c>
@@ -5392,13 +5374,13 @@
         <v>-1.7278677084930461</v>
       </c>
       <c r="O90">
-        <v>-1.888889008994302</v>
+        <v>-1.761995001543794</v>
       </c>
       <c r="P90">
         <v>-1.9535200610362209</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="91">
       <c r="A91" t="s">
         <v>137</v>
       </c>
@@ -5442,13 +5424,13 @@
         <v>-2.839065243022461</v>
       </c>
       <c r="O91">
-        <v>-3.560036637817773</v>
+        <v>-2.2991768927130232</v>
       </c>
       <c r="P91">
         <v>-3.2621539915251092</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="92">
       <c r="A92" t="s">
         <v>67</v>
       </c>
@@ -5492,13 +5474,13 @@
         <v>-2.5032410617151002</v>
       </c>
       <c r="O92">
-        <v>-3.276025622554219</v>
+        <v>-1.9340209619469131</v>
       </c>
       <c r="P92">
         <v>-3.8297794554954292</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="93">
       <c r="A93" t="s">
         <v>41</v>
       </c>
@@ -5542,13 +5524,13 @@
         <v>-1.7526066847539139</v>
       </c>
       <c r="O93">
-        <v>-1.923017801874819</v>
+        <v>-1.896026509636713</v>
       </c>
       <c r="P93">
         <v>-2.190151549272946</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="94">
       <c r="A94" t="s">
         <v>51</v>
       </c>
@@ -5592,13 +5574,13 @@
         <v>-1.775576249517945</v>
       </c>
       <c r="O94">
-        <v>-2.000421963789123</v>
+        <v>-1.5834650294452299</v>
       </c>
       <c r="P94">
         <v>-2.2209390605344912</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="95">
       <c r="A95" t="s">
         <v>146</v>
       </c>
@@ -5642,13 +5624,13 @@
         <v>-1.5378203504490739</v>
       </c>
       <c r="O95">
-        <v>-1.756281665942053</v>
+        <v>-2.1518223022991601</v>
       </c>
       <c r="P95">
         <v>-1.8386531269014319</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="96">
       <c r="A96" t="s">
         <v>79</v>
       </c>
@@ -5692,13 +5674,13 @@
         <v>-2.0316149962873569</v>
       </c>
       <c r="O96">
-        <v>-2.3457625400034261</v>
+        <v>-1.0385124687186651</v>
       </c>
       <c r="P96">
         <v>-2.0638469813864688</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="97">
       <c r="A97" t="s">
         <v>1</v>
       </c>
@@ -5742,13 +5724,13 @@
         <v>-1.7855693218914599</v>
       </c>
       <c r="O97">
-        <v>-2.5638043529732282</v>
+        <v>-1.4551041270718681</v>
       </c>
       <c r="P97">
         <v>-2.9703337071434062</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="98">
       <c r="A98" t="s">
         <v>56</v>
       </c>
@@ -5792,13 +5774,13 @@
         <v>-0.93778902373218687</v>
       </c>
       <c r="O98">
-        <v>-0.86795587885461012</v>
+        <v>-1.881905889801972</v>
       </c>
       <c r="P98">
         <v>-0.63019682725801895</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="99">
       <c r="A99" t="s">
         <v>85</v>
       </c>
@@ -5842,13 +5824,13 @@
         <v>-0.96761469518338961</v>
       </c>
       <c r="O99">
-        <v>-1.4982244064000521</v>
+        <v>-3.006878062117893</v>
       </c>
       <c r="P99">
         <v>-1.5030601131724231</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="100">
       <c r="A100" t="s">
         <v>69</v>
       </c>
@@ -5892,13 +5874,13 @@
         <v>-0.33302747546663758</v>
       </c>
       <c r="O100">
-        <v>0.2279088621277465</v>
+        <v>-16.128387224167788</v>
       </c>
       <c r="P100">
         <v>0.22222879134266399</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="101">
       <c r="A101" t="s">
         <v>107</v>
       </c>
@@ -5942,13 +5924,13 @@
         <v>-1.176287544783144</v>
       </c>
       <c r="O101">
-        <v>-1.4024509000222489</v>
+        <v>-2.234557968804844</v>
       </c>
       <c r="P101">
         <v>-1.8506580627239131</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="102">
       <c r="A102" t="s">
         <v>89</v>
       </c>
@@ -5992,13 +5974,13 @@
         <v>-1.563496712483105</v>
       </c>
       <c r="O102">
-        <v>-1.761995001543794</v>
+        <v>-1.3789843028809601</v>
       </c>
       <c r="P102">
         <v>-1.4785583497952299</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="103">
       <c r="A103" t="s">
         <v>145</v>
       </c>
@@ -6042,13 +6024,13 @@
         <v>-1.616153132387403</v>
       </c>
       <c r="O103">
-        <v>-1.5685355309425619</v>
+        <v>-1.602659131324522</v>
       </c>
       <c r="P103">
         <v>-2.1638386472455888</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="104">
       <c r="A104" t="s">
         <v>22</v>
       </c>
@@ -6092,13 +6074,13 @@
         <v>-1.5107988394022891</v>
       </c>
       <c r="O104">
-        <v>-1.498301796825479</v>
+        <v>-2.807380829680707</v>
       </c>
       <c r="P104">
         <v>-1.311981369440685</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="105">
       <c r="A105" t="s">
         <v>126</v>
       </c>
@@ -6142,13 +6124,13 @@
         <v>-1.45360186070572</v>
       </c>
       <c r="O105">
-        <v>-1.4580332051604461</v>
+        <v>-1.5142493606996721</v>
       </c>
       <c r="P105">
         <v>-1.815757794045527</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="106">
       <c r="A106" t="s">
         <v>93</v>
       </c>
@@ -6192,13 +6174,13 @@
         <v>-1.4128597193622541</v>
       </c>
       <c r="O106">
-        <v>-1.5834650294452299</v>
+        <v>-3.1557623644588721</v>
       </c>
       <c r="P106">
         <v>-1.760379171033106</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="107">
       <c r="A107" t="s">
         <v>30</v>
       </c>
@@ -6242,13 +6224,13 @@
         <v>-1.2801691245287601</v>
       </c>
       <c r="O107">
-        <v>-1.308767918691963</v>
+        <v>-2.131620143027297</v>
       </c>
       <c r="P107">
         <v>-1.5388733732449409</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="108">
       <c r="A108" t="s">
         <v>96</v>
       </c>
@@ -6292,13 +6274,13 @@
         <v>-1.177219092709761</v>
       </c>
       <c r="O108">
-        <v>-1.4551041270718681</v>
+        <v>-1.4024509000222489</v>
       </c>
       <c r="P108">
         <v>-1.008683919487011</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="109">
       <c r="A109" t="s">
         <v>78</v>
       </c>
@@ -6342,13 +6324,13 @@
         <v>-1.737424363382523</v>
       </c>
       <c r="O109">
-        <v>-1.9961549048662059</v>
+        <v>-1.1073908193552751</v>
       </c>
       <c r="P109">
         <v>-2.663810038699467</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="110">
       <c r="A110" t="s">
         <v>66</v>
       </c>
@@ -6392,13 +6374,13 @@
         <v>-1.3537870783933741</v>
       </c>
       <c r="O110">
-        <v>-1.4166974892347779</v>
+        <v>-1.836818521304274</v>
       </c>
       <c r="P110">
         <v>-1.4301140844131901</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="111">
       <c r="A111" t="s">
         <v>54</v>
       </c>
@@ -6442,13 +6424,13 @@
         <v>-1.118744349809609</v>
       </c>
       <c r="O111">
-        <v>-0.57679142768196268</v>
+        <v>-1.3843378691300201</v>
       </c>
       <c r="P111">
         <v>-0.12580935490473191</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="112">
       <c r="A112" t="s">
         <v>53</v>
       </c>
@@ -6492,13 +6474,13 @@
         <v>-1.5478940322029371</v>
       </c>
       <c r="O112">
-        <v>-1.882344554530639</v>
+        <v>-1.3285220151799779</v>
       </c>
       <c r="P112">
         <v>-1.946531498702726</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="113">
       <c r="A113" t="s">
         <v>15</v>
       </c>
@@ -6542,13 +6524,13 @@
         <v>-0.88844471194424357</v>
       </c>
       <c r="O113">
-        <v>-1.0794431210827149</v>
+        <v>-1.152911611315341</v>
       </c>
       <c r="P113">
         <v>-1.594165768002153</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="114">
       <c r="A114" t="s">
         <v>140</v>
       </c>
@@ -6592,13 +6574,13 @@
         <v>-2.0533777939005109</v>
       </c>
       <c r="O114">
-        <v>-2.1436228820040348</v>
+        <v>-2.6341214830080371</v>
       </c>
       <c r="P114">
         <v>-2.5719856398815182</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="115">
       <c r="A115" t="s">
         <v>110</v>
       </c>
@@ -6642,13 +6624,13 @@
         <v>-0.85389166173598396</v>
       </c>
       <c r="O115">
-        <v>-1.3843378691300201</v>
+        <v>-2.112233498473584</v>
       </c>
       <c r="P115">
         <v>-0.93911660449802703</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="116">
       <c r="A116" t="s">
         <v>9</v>
       </c>
@@ -6692,13 +6674,13 @@
         <v>-1.722673219878019</v>
       </c>
       <c r="O116">
-        <v>-2.0599921269573329</v>
+        <v>-2.2776806176397701</v>
       </c>
       <c r="P116">
         <v>-2.066248714121429</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="117">
       <c r="A117" t="s">
         <v>13</v>
       </c>
@@ -6742,13 +6724,13 @@
         <v>-0.5847812385135932</v>
       </c>
       <c r="O117">
-        <v>-0.58521144759678034</v>
+        <v>-2.619289920597569</v>
       </c>
       <c r="P117">
         <v>-0.68577214351885607</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="118">
       <c r="A118" t="s">
         <v>104</v>
       </c>
@@ -6792,13 +6774,13 @@
         <v>-1.3000651075978431</v>
       </c>
       <c r="O118">
-        <v>-1.5142493606996721</v>
+        <v>-3.9450832163289009</v>
       </c>
       <c r="P118">
         <v>-1.6788066622347531</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="119">
       <c r="A119" t="s">
         <v>101</v>
       </c>
@@ -6842,13 +6824,13 @@
         <v>-1.435434539889477</v>
       </c>
       <c r="O119">
-        <v>-1.3789843028809601</v>
+        <v>-2.0358653776459068</v>
       </c>
       <c r="P119">
         <v>-0.21646614339886069</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="120">
       <c r="A120" t="s">
         <v>109</v>
       </c>
@@ -6892,13 +6874,13 @@
         <v>-1.615969126525119</v>
       </c>
       <c r="O120">
-        <v>-1.836818521304274</v>
+        <v>-1.339914478594993</v>
       </c>
       <c r="P120">
         <v>-2.0144514360103138</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="121">
       <c r="A121" t="s">
         <v>125</v>
       </c>
@@ -6942,13 +6924,13 @@
         <v>-1.2811267156215389</v>
       </c>
       <c r="O121">
-        <v>-1.496797327314574</v>
+        <v>-6.0613666365157206</v>
       </c>
       <c r="P121">
         <v>-1.7488835052818421</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="122">
       <c r="A122" t="s">
         <v>63</v>
       </c>
@@ -6992,13 +6974,13 @@
         <v>-0.51400893763050215</v>
       </c>
       <c r="O122">
-        <v>-0.46892191352523233</v>
+        <v>-2.1994665822257979</v>
       </c>
       <c r="P122">
         <v>-0.73341471016347604</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="123">
       <c r="A123" t="s">
         <v>118</v>
       </c>
@@ -7042,13 +7024,13 @@
         <v>-1.628555303572804</v>
       </c>
       <c r="O123">
-        <v>-2.0358653776459068</v>
+        <v>-2.056949524355498</v>
       </c>
       <c r="P123">
         <v>-2.0030954014337929</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="124">
       <c r="A124" t="s">
         <v>119</v>
       </c>
@@ -7092,13 +7074,13 @@
         <v>-0.9909352626353426</v>
       </c>
       <c r="O124">
-        <v>-1.339914478594993</v>
+        <v>0.31924638912835213</v>
       </c>
       <c r="P124">
         <v>-1.404129894706843</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="125">
       <c r="A125" t="s">
         <v>111</v>
       </c>
@@ -7142,13 +7124,13 @@
         <v>-1.0665420280041229</v>
       </c>
       <c r="O125">
-        <v>-1.3285220151799779</v>
+        <v>-2.1948338957660471</v>
       </c>
       <c r="P125">
         <v>-1.3774198990645741</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="126">
       <c r="A126" t="s">
         <v>112</v>
       </c>
@@ -7192,13 +7174,13 @@
         <v>-1.024962041849345</v>
       </c>
       <c r="O126">
-        <v>-1.152911611315341</v>
+        <v>-1.496797327314574</v>
       </c>
       <c r="P126">
         <v>-1.1127852092717709</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="127">
       <c r="A127" t="s">
         <v>64</v>
       </c>
@@ -7242,13 +7224,13 @@
         <v>-1.3679500066386949</v>
       </c>
       <c r="O127">
-        <v>-1.5292953896156209</v>
+        <v>-1.4580332051604461</v>
       </c>
       <c r="P127">
         <v>-1.7613601390977141</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="128">
       <c r="A128" t="s">
         <v>49</v>
       </c>
@@ -7292,13 +7274,13 @@
         <v>-0.51123818970109292</v>
       </c>
       <c r="O128">
-        <v>-0.81815043665245191</v>
+        <v>-1.1303461262420711</v>
       </c>
       <c r="P128">
         <v>-0.81384405976116136</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="129">
       <c r="A129" t="s">
         <v>95</v>
       </c>
@@ -7342,13 +7324,13 @@
         <v>-0.84691284969636604</v>
       </c>
       <c r="O129">
-        <v>-1.0385124687186651</v>
+        <v>-5.8972549820172491</v>
       </c>
       <c r="P129">
         <v>-1.9255408721722069</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="130">
       <c r="A130" t="s">
         <v>52</v>
       </c>
@@ -7392,13 +7374,13 @@
         <v>-0.69312168773691718</v>
       </c>
       <c r="O130">
-        <v>-0.83575044073620497</v>
+        <v>-2.1514519230217051</v>
       </c>
       <c r="P130">
         <v>-1.3107354763209691</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="131">
       <c r="A131" t="s">
         <v>16</v>
       </c>
@@ -7442,13 +7424,13 @@
         <v>-0.55650878717401109</v>
       </c>
       <c r="O131">
-        <v>-0.79047591821232599</v>
+        <v>-2.1690494492313031</v>
       </c>
       <c r="P131">
         <v>-0.89811822869019509</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="132">
       <c r="A132" t="s">
         <v>138</v>
       </c>
@@ -7492,13 +7474,13 @@
         <v>-1.26714945345208</v>
       </c>
       <c r="O132">
-        <v>-1.5924099781167029</v>
+        <v>-12.124795192440899</v>
       </c>
       <c r="P132">
         <v>-1.628826605088928</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="133">
       <c r="A133" t="s">
         <v>82</v>
       </c>
@@ -7542,13 +7524,13 @@
         <v>-1.2320574270440949</v>
       </c>
       <c r="O133">
-        <v>-1.178253605740319</v>
+        <v>-1.881898909100997</v>
       </c>
       <c r="P133">
         <v>-0.84161782182377842</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="134">
       <c r="A134" t="s">
         <v>61</v>
       </c>
@@ -7592,13 +7574,13 @@
         <v>-1.5453339440093821</v>
       </c>
       <c r="O134">
-        <v>-1.884701478940177</v>
+        <v>-2.7585320079900182</v>
       </c>
       <c r="P134">
         <v>-2.0218768123547681</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="135">
       <c r="A135" t="s">
         <v>35</v>
       </c>
@@ -7642,13 +7624,13 @@
         <v>-0.34573290484140062</v>
       </c>
       <c r="O135">
-        <v>-0.59645923001078116</v>
+        <v>-2.4996639170257571</v>
       </c>
       <c r="P135">
         <v>-1.339398089551519</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="136">
       <c r="A136" t="s">
         <v>122</v>
       </c>
@@ -7692,13 +7674,13 @@
         <v>-1.6038643671571211</v>
       </c>
       <c r="O136">
-        <v>-2.056949524355498</v>
+        <v>-0.78220285780793741</v>
       </c>
       <c r="P136">
         <v>-2.1439345419139291</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="137">
       <c r="A137" t="s">
         <v>108</v>
       </c>
@@ -7742,13 +7724,13 @@
         <v>-0.72765737974401346</v>
       </c>
       <c r="O137">
-        <v>-1.1073908193552751</v>
+        <v>-4.8164369576977446</v>
       </c>
       <c r="P137">
         <v>-1.1526821894438419</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="138">
       <c r="A138" t="s">
         <v>29</v>
       </c>
@@ -7792,13 +7774,13 @@
         <v>-0.7535605321076968</v>
       </c>
       <c r="O138">
-        <v>-1.1084819198036899</v>
+        <v>-3.560036637817773</v>
       </c>
       <c r="P138">
         <v>-1.482438270809372</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="139">
       <c r="A139" t="s">
         <v>38</v>
       </c>
@@ -7842,13 +7824,13 @@
         <v>-0.66004856847819671</v>
       </c>
       <c r="O139">
-        <v>-0.99079914278383074</v>
+        <v>-1.5924099781167029</v>
       </c>
       <c r="P139">
         <v>-1.2157176008197359</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="140">
       <c r="A140" t="s">
         <v>143</v>
       </c>
@@ -7892,13 +7874,13 @@
         <v>-0.5211362713638259</v>
       </c>
       <c r="O140">
-        <v>-0.34066288367558573</v>
+        <v>-2.5160300971999372</v>
       </c>
       <c r="P140">
         <v>-0.35559190225365611</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="141">
       <c r="A141" t="s">
         <v>10</v>
       </c>
@@ -7942,13 +7924,13 @@
         <v>-0.33653688249472102</v>
       </c>
       <c r="O141">
-        <v>-0.58885984623404464</v>
+        <v>-2.1436228820040348</v>
       </c>
       <c r="P141">
         <v>-0.58027132390672065</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="142">
       <c r="A142" t="s">
         <v>135</v>
       </c>
@@ -7992,13 +7974,13 @@
         <v>-0.39395909505506271</v>
       </c>
       <c r="O142">
-        <v>-0.78220285780793741</v>
+        <v>-1.888889008994302</v>
       </c>
       <c r="P142">
         <v>-0.68962004563607848</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="143">
       <c r="A143" t="s">
         <v>58</v>
       </c>
@@ -8042,13 +8024,13 @@
         <v>-0.84208158423542889</v>
       </c>
       <c r="O143">
-        <v>-1.552935003874216</v>
+        <v>-3.538723149636597</v>
       </c>
       <c r="P143">
         <v>-1.9948718792960789</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="144">
       <c r="A144" t="s">
         <v>76</v>
       </c>
@@ -8092,13 +8074,13 @@
         <v>-0.78245470346262425</v>
       </c>
       <c r="O144">
-        <v>-1.258331271851314</v>
+        <v>-0.34066288367558573</v>
       </c>
       <c r="P144">
         <v>-2.0141185661318071</v>
       </c>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="145">
       <c r="A145" t="s">
         <v>123</v>
       </c>
@@ -8142,13 +8124,13 @@
         <v>0.72851423541127514</v>
       </c>
       <c r="O145">
-        <v>0.31924638912835213</v>
+        <v>-2.2091532010369912</v>
       </c>
       <c r="P145">
         <v>6.2847544670487407E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="146">
       <c r="A146" t="s">
         <v>8</v>
       </c>
@@ -8192,13 +8174,13 @@
         <v>1.065300595355388</v>
       </c>
       <c r="O146">
-        <v>1.1896713589043659</v>
+        <v>-1.5685355309425619</v>
       </c>
       <c r="P146">
         <v>1.043506196850053</v>
       </c>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="147">
       <c r="A147" t="s">
         <v>17</v>
       </c>
@@ -8242,7 +8224,7 @@
         <v>-0.13842627831749921</v>
       </c>
       <c r="O147">
-        <v>-0.69620251389204446</v>
+        <v>-1.756281665942053</v>
       </c>
       <c r="P147">
         <v>-1.021956367882775</v>
@@ -8270,16 +8252,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P147"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="false" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8329,7 +8311,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -8379,7 +8361,7 @@
         <v>-3.1433970500850399</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -8429,7 +8411,7 @@
         <v>-1.3397854870801049</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -8479,7 +8461,7 @@
         <v>-1.403855318995707</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -8529,7 +8511,7 @@
         <v>-1.88212710492705</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -8579,7 +8561,7 @@
         <v>-2.21675742179207</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -8629,7 +8611,7 @@
         <v>-2.3336456843901501</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -8679,7 +8661,7 @@
         <v>-1.047490719653466</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -8729,7 +8711,7 @@
         <v>0.93899051481842377</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -8779,7 +8761,7 @@
         <v>-2.1781641716181599</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -8829,7 +8811,7 @@
         <v>-0.40399437579789532</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -8879,7 +8861,7 @@
         <v>-2.3944524403693048</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -8929,7 +8911,7 @@
         <v>-2.2834514334153062</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -8979,7 +8961,7 @@
         <v>-1.5059794845421259</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -9029,7 +9011,7 @@
         <v>-1.7279873676869439</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -9079,7 +9061,7 @@
         <v>-1.464229202642757</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -9129,7 +9111,7 @@
         <v>-0.72893886462322233</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -9179,7 +9161,7 @@
         <v>-1.026559724010945</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -9229,7 +9211,7 @@
         <v>-1.146513179767634</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -9279,7 +9261,7 @@
         <v>-2.2152589626258421</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -9329,7 +9311,7 @@
         <v>-2.3461069239870009</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -9379,7 +9361,7 @@
         <v>-1.087279465151459</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -9429,7 +9411,7 @@
         <v>-3.8728686786278401</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -9479,7 +9461,7 @@
         <v>-1.7150441712649069</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -9529,7 +9511,7 @@
         <v>-1.513817142315466</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -9579,7 +9561,7 @@
         <v>-2.0559200314127581</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -9629,7 +9611,7 @@
         <v>0.17636436048790621</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -9679,7 +9661,7 @@
         <v>-2.0726104232734559</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -9729,7 +9711,7 @@
         <v>-1.2482988302030029</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -9779,7 +9761,7 @@
         <v>-1.3803954937058081</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -9829,7 +9811,7 @@
         <v>-1.230636766412287</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -9879,7 +9861,7 @@
         <v>-4.0137534808828814</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -9929,7 +9911,7 @@
         <v>-1.3065584427368151</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -9979,7 +9961,7 @@
         <v>-1.0636839321228651</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -10029,7 +10011,7 @@
         <v>-1.6784148432609991</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -10079,7 +10061,7 @@
         <v>-1.246396036250456</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -10129,7 +10111,7 @@
         <v>-1.875762516824943</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -10179,7 +10161,7 @@
         <v>-1.9234146814685189</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -10229,7 +10211,7 @@
         <v>-1.3608743994474251</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -10279,7 +10261,7 @@
         <v>-2.241275246529757</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -10329,7 +10311,7 @@
         <v>-1.4329619319271341</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -10379,7 +10361,7 @@
         <v>-1.786472611977973</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -10429,7 +10411,7 @@
         <v>-2.1930475222656129</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -10479,7 +10461,7 @@
         <v>-2.3737842376578611</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -10529,7 +10511,7 @@
         <v>-2.0506058662857272</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -10579,7 +10561,7 @@
         <v>-1.061139229572299</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -10629,7 +10611,7 @@
         <v>-1.7349930922650889</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -10679,7 +10661,7 @@
         <v>-1.1386377201858451</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -10729,7 +10711,7 @@
         <v>-1.934400198192852</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -10779,7 +10761,7 @@
         <v>-0.99419321827449658</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -10829,7 +10811,7 @@
         <v>-1.438187888053557</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -10879,7 +10861,7 @@
         <v>-2.5998335690383301</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -10929,7 +10911,7 @@
         <v>-1.2049005294039441</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -10979,7 +10961,7 @@
         <v>-1.744513718321391</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -11029,7 +11011,7 @@
         <v>3.5913933014881702E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -11079,7 +11061,7 @@
         <v>-0.72497453763464814</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -11129,7 +11111,7 @@
         <v>-4.8365727691564199E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -11179,7 +11161,7 @@
         <v>-2.1434215440651219</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -11229,7 +11211,7 @@
         <v>-1.847325849505284</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -11279,7 +11261,7 @@
         <v>-1.992474270163894</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -11329,7 +11311,7 @@
         <v>-1.7354027662164559</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -11379,7 +11361,7 @@
         <v>-2.021284197349182</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -11429,7 +11411,7 @@
         <v>-2.6639128892561641</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="64">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -11479,7 +11461,7 @@
         <v>-0.70292115113425668</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -11529,7 +11511,7 @@
         <v>-1.5513828975318</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="66">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -11579,7 +11561,7 @@
         <v>-2.8373617851813679</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="67">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -11629,7 +11611,7 @@
         <v>-1.642999613155002</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="68">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -11679,7 +11661,7 @@
         <v>-3.7874721996834402</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="69">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -11729,7 +11711,7 @@
         <v>-1.1556795047694219</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="70">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -11779,7 +11761,7 @@
         <v>-0.26035459606480738</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="71">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -11829,7 +11811,7 @@
         <v>-1.4863448898978311</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="72">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -11879,7 +11861,7 @@
         <v>-1.591917493684587</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="73">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -11929,7 +11911,7 @@
         <v>-2.3101427683985092</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="74">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -11979,7 +11961,7 @@
         <v>-0.9395133471975794</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="75">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -12029,7 +12011,7 @@
         <v>-1.273874927687453</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="76">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -12079,7 +12061,7 @@
         <v>-2.6753276155017578</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="77">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -12129,7 +12111,7 @@
         <v>-2.157728738545313</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="78">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -12179,7 +12161,7 @@
         <v>-2.5231562522048181</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="79">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -12229,7 +12211,7 @@
         <v>-2.521088624252259</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="80">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -12279,7 +12261,7 @@
         <v>-1.916900262230103</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="81">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -12329,7 +12311,7 @@
         <v>-0.65397192744952704</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="82">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -12379,7 +12361,7 @@
         <v>-2.252207405428353</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="83">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -12429,7 +12411,7 @@
         <v>-0.73690921337505699</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="84">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -12479,7 +12461,7 @@
         <v>-2.3549813068795942</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="85">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -12529,7 +12511,7 @@
         <v>-1.457975123855916</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="86">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -12579,7 +12561,7 @@
         <v>-0.94221946938970547</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="87">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -12629,7 +12611,7 @@
         <v>-1.916527194071926</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="88">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -12679,7 +12661,7 @@
         <v>-1.1491342260772119</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="89">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -12729,7 +12711,7 @@
         <v>-5.3632959136438503</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="90">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -12779,7 +12761,7 @@
         <v>-1.5296834265945569</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="91">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -12829,7 +12811,7 @@
         <v>-2.1039871566473809</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="92">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -12879,7 +12861,7 @@
         <v>-1.729205499209679</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="93">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -12929,7 +12911,7 @@
         <v>-1.548581894681385</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="94">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -12979,7 +12961,7 @@
         <v>-1.4447718122757609</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="95">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -13029,7 +13011,7 @@
         <v>-2.1237023903768661</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="96">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -13079,7 +13061,7 @@
         <v>-1.682065229057639</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="97">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -13129,7 +13111,7 @@
         <v>-1.210560511023228</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="98">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -13179,7 +13161,7 @@
         <v>-0.71322495354138971</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="99">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -13229,7 +13211,7 @@
         <v>-2.3941456590386059</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="100">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -13279,7 +13261,7 @@
         <v>-1.8910529183374609</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="101">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -13329,7 +13311,7 @@
         <v>-1.8606762393923431</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="102">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -13379,7 +13361,7 @@
         <v>-1.454791577159734</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="103">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -13429,7 +13411,7 @@
         <v>-2.4332356105208901</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="104">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -13479,7 +13461,7 @@
         <v>-2.781736907967983</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="105">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -13529,7 +13511,7 @@
         <v>-1.5557257969473131</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="106">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -13579,7 +13561,7 @@
         <v>-2.047118426712998</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="107">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -13629,7 +13611,7 @@
         <v>-1.461950747286308</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="108">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -13679,7 +13661,7 @@
         <v>-1.7069393839355429</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="109">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -13729,7 +13711,7 @@
         <v>-2.0456328268412278</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="110">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -13779,7 +13761,7 @@
         <v>-1.9991632526108449</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="111">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -13829,7 +13811,7 @@
         <v>-0.78834299413188624</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="112">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -13879,7 +13861,7 @@
         <v>-1.315106769294677</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="113">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -13929,7 +13911,7 @@
         <v>-1.2872633061353489</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="114">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -13979,7 +13961,7 @@
         <v>-1.36083366943844</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="115">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -14029,7 +14011,7 @@
         <v>-1.563752243052748</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="116">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -14079,7 +14061,7 @@
         <v>-2.1930946672648188</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="117">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -14129,7 +14111,7 @@
         <v>-2.1686492571292799</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="118">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -14179,7 +14161,7 @@
         <v>-2.726542705995485</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="119">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -14229,7 +14211,7 @@
         <v>-2.0069158259045579</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="120">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -14279,7 +14261,7 @@
         <v>-1.396698283086883</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="121">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -14329,7 +14311,7 @@
         <v>-2.9721609006417138</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="122">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -14379,7 +14361,7 @@
         <v>-1.8060402893989009</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="123">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -14429,7 +14411,7 @@
         <v>-2.3413065292596711</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="124">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -14479,7 +14461,7 @@
         <v>7.0266754953168906E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="125">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -14529,7 +14511,7 @@
         <v>-1.9979509762020731</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="126">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -14579,7 +14561,7 @@
         <v>-1.644831231212474</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="127">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -14629,7 +14611,7 @@
         <v>-2.0977260641446578</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="128">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -14679,7 +14661,7 @@
         <v>-1.4089767988166511</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="129">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -14729,7 +14711,7 @@
         <v>-3.7104559677917588</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="130">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -14779,7 +14761,7 @@
         <v>-1.023101434434472</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="131">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -14829,7 +14811,7 @@
         <v>-1.555710728751116</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="132">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -14879,7 +14861,7 @@
         <v>-1.620237793438851</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="133">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -14929,7 +14911,7 @@
         <v>-1.381953330200931</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="134">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -14979,7 +14961,7 @@
         <v>-1.249570997903245</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="135">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -15029,7 +15011,7 @@
         <v>-1.898237653312149</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="136">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -15079,7 +15061,7 @@
         <v>-1.1438525768443759</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="137">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -15129,7 +15111,7 @@
         <v>-4.8630370600766533</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="138">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -15179,7 +15161,7 @@
         <v>-2.7470851239922029</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="139">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -15229,7 +15211,7 @@
         <v>-1.774374802299691</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="140">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -15279,7 +15261,7 @@
         <v>-2.2748344556061291</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="141">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -15329,7 +15311,7 @@
         <v>-2.5217848442788098</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="142">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -15379,7 +15361,7 @@
         <v>-1.599254698748215</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="143">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -15429,7 +15411,7 @@
         <v>-2.1293043248483441</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="144">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -15479,7 +15461,7 @@
         <v>-5.3187544900134102E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="145">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -15529,7 +15511,7 @@
         <v>-0.43503422732097757</v>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="146">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -15579,7 +15561,7 @@
         <v>-1.9347931596176151</v>
       </c>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="147">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -15640,744 +15622,744 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="P1:P147"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="false" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="P1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="P2">
         <v>-3.1057715026790569</v>
       </c>
     </row>
-    <row r="3" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="P3">
         <v>-1.487594326238143</v>
       </c>
     </row>
-    <row r="4" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="P4">
         <v>-1.819122924667381</v>
       </c>
     </row>
-    <row r="5" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="P5">
         <v>-1.786007137889231</v>
       </c>
     </row>
-    <row r="6" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="P6">
         <v>-2.09930651177782</v>
       </c>
     </row>
-    <row r="7" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="P7">
         <v>-1.672869634846492</v>
       </c>
     </row>
-    <row r="8" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="P8">
         <v>-1.7226865089241981</v>
       </c>
     </row>
-    <row r="9" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="P9">
         <v>-0.76010426222809924</v>
       </c>
     </row>
-    <row r="10" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="P10">
         <v>-4.3023791514390073</v>
       </c>
     </row>
-    <row r="11" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="P11">
         <v>-0.29937525828725731</v>
       </c>
     </row>
-    <row r="12" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="P12">
         <v>-1.899081484564088</v>
       </c>
     </row>
-    <row r="13" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="P13">
         <v>-1.8400766255050021</v>
       </c>
     </row>
-    <row r="14" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="P14">
         <v>-1.401684762237855</v>
       </c>
     </row>
-    <row r="15" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="P15">
         <v>-1.831294551174647</v>
       </c>
     </row>
-    <row r="16" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="P16">
         <v>-1.3592934361542679</v>
       </c>
     </row>
-    <row r="17" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="P17">
         <v>-0.27377300547823818</v>
       </c>
     </row>
-    <row r="18" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="P18">
         <v>-12.29512691952937</v>
       </c>
     </row>
-    <row r="19" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="P19">
         <v>-0.7031159021156187</v>
       </c>
     </row>
-    <row r="20" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="P20">
         <v>-2.4260247270093478</v>
       </c>
     </row>
-    <row r="21" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="P21">
         <v>-1.991317178869316</v>
       </c>
     </row>
-    <row r="22" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="P22">
         <v>-1.323826372492255</v>
       </c>
     </row>
-    <row r="23" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="P23">
         <v>-1.9290088784753849</v>
       </c>
     </row>
-    <row r="24" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="P24">
         <v>-1.432322309651574</v>
       </c>
     </row>
-    <row r="25" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="P25">
         <v>-1.8985664878935291</v>
       </c>
     </row>
-    <row r="26" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="P26">
         <v>-1.867353488707266</v>
       </c>
     </row>
-    <row r="27" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="P27">
         <v>-2.3200022987068061</v>
       </c>
     </row>
-    <row r="28" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="P28">
         <v>-1.837316843105365</v>
       </c>
     </row>
-    <row r="29" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="P29">
         <v>-1.809489340650053</v>
       </c>
     </row>
-    <row r="30" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="P30">
         <v>-1.2764913926767329</v>
       </c>
     </row>
-    <row r="31" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="P31">
         <v>-1.037404624274735</v>
       </c>
     </row>
-    <row r="32" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="P32">
         <v>-0.92449298796848323</v>
       </c>
     </row>
-    <row r="33" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="33">
       <c r="P33">
         <v>-1.0012557327432889</v>
       </c>
     </row>
-    <row r="34" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="34">
       <c r="P34">
         <v>-1.298289013008219</v>
       </c>
     </row>
-    <row r="35" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="35">
       <c r="P35">
         <v>-0.75337135551124046</v>
       </c>
     </row>
-    <row r="36" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="36">
       <c r="P36">
         <v>-2.045253191451522</v>
       </c>
     </row>
-    <row r="37" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="37">
       <c r="P37">
         <v>-1.07162256296748</v>
       </c>
     </row>
-    <row r="38" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="38">
       <c r="P38">
         <v>-1.7741167369851789</v>
       </c>
     </row>
-    <row r="39" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="39">
       <c r="P39">
         <v>-1.6101152865985919</v>
       </c>
     </row>
-    <row r="40" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="40">
       <c r="P40">
         <v>-1.0363665392411541</v>
       </c>
     </row>
-    <row r="41" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="41">
       <c r="P41">
         <v>-2.1477572064080208</v>
       </c>
     </row>
-    <row r="42" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="42">
       <c r="P42">
         <v>-1.4905201079729991</v>
       </c>
     </row>
-    <row r="43" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="43">
       <c r="P43">
         <v>-9.5910643250753633</v>
       </c>
     </row>
-    <row r="44" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="44">
       <c r="P44">
         <v>-2.5068991930896138</v>
       </c>
     </row>
-    <row r="45" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="45">
       <c r="P45">
         <v>-1.9933867100735929</v>
       </c>
     </row>
-    <row r="46" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="46">
       <c r="P46">
         <v>-1.8516053686060869</v>
       </c>
     </row>
-    <row r="47" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="47">
       <c r="P47">
         <v>-1.8942606877735511</v>
       </c>
     </row>
-    <row r="48" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="48">
       <c r="P48">
         <v>-0.72457914318743788</v>
       </c>
     </row>
-    <row r="49" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="49">
       <c r="P49">
         <v>-1.6371852125687021</v>
       </c>
     </row>
-    <row r="50" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="50">
       <c r="P50">
         <v>-1.266302728499394</v>
       </c>
     </row>
-    <row r="51" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="51">
       <c r="P51">
         <v>-1.986899163173879</v>
       </c>
     </row>
-    <row r="52" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="52">
       <c r="P52">
         <v>-1.2134198053144101</v>
       </c>
     </row>
-    <row r="53" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="53">
       <c r="P53">
         <v>-2.101151222867589</v>
       </c>
     </row>
-    <row r="54" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="54">
       <c r="P54">
         <v>-1.418678573923112</v>
       </c>
     </row>
-    <row r="55" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="55">
       <c r="P55">
         <v>-2.8121172216019339</v>
       </c>
     </row>
-    <row r="56" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="56">
       <c r="P56">
         <v>-3.2144623432943451</v>
       </c>
     </row>
-    <row r="57" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="57">
       <c r="P57">
         <v>-1.069514849298226</v>
       </c>
     </row>
-    <row r="58" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="58">
       <c r="P58">
         <v>-1.583201856934227</v>
       </c>
     </row>
-    <row r="59" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="59">
       <c r="P59">
         <v>-1.0405209736102781</v>
       </c>
     </row>
-    <row r="60" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="60">
       <c r="P60">
         <v>-1.135330456008151</v>
       </c>
     </row>
-    <row r="61" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="61">
       <c r="P61">
         <v>-1.8480136850537849</v>
       </c>
     </row>
-    <row r="62" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="62">
       <c r="P62">
         <v>-2.7152690949087441</v>
       </c>
     </row>
-    <row r="63" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="63">
       <c r="P63">
         <v>-2.529500402660108</v>
       </c>
     </row>
-    <row r="64" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="64">
       <c r="P64">
         <v>-0.45453295182363501</v>
       </c>
     </row>
-    <row r="65" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="65">
       <c r="P65">
         <v>-1.193972516771092</v>
       </c>
     </row>
-    <row r="66" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="66">
       <c r="P66">
         <v>-3.026287454561376</v>
       </c>
     </row>
-    <row r="67" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="67">
       <c r="P67">
         <v>-3.460161458531712</v>
       </c>
     </row>
-    <row r="68" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="68">
       <c r="P68">
         <v>-3.497168490021191</v>
       </c>
     </row>
-    <row r="69" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="69">
       <c r="P69">
         <v>-2.086172891733916</v>
       </c>
     </row>
-    <row r="70" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="70">
       <c r="P70">
         <v>-1.579563852517573</v>
       </c>
     </row>
-    <row r="71" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="71">
       <c r="P71">
         <v>-2.2488011646966419</v>
       </c>
     </row>
-    <row r="72" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="72">
       <c r="P72">
         <v>-2.0721108162581832</v>
       </c>
     </row>
-    <row r="73" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="73">
       <c r="P73">
         <v>-2.0833912199751121</v>
       </c>
     </row>
-    <row r="74" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="74">
       <c r="P74">
         <v>-0.52402706722416936</v>
       </c>
     </row>
-    <row r="75" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="75">
       <c r="P75">
         <v>-0.89912561504852151</v>
       </c>
     </row>
-    <row r="76" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="76">
       <c r="P76">
         <v>-1.2574437717835369</v>
       </c>
     </row>
-    <row r="77" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="77">
       <c r="P77">
         <v>-1.9541023365953509</v>
       </c>
     </row>
-    <row r="78" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="78">
       <c r="P78">
         <v>-2.0729074270788641</v>
       </c>
     </row>
-    <row r="79" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="79">
       <c r="P79">
         <v>-2.648006483433329</v>
       </c>
     </row>
-    <row r="80" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="80">
       <c r="P80">
         <v>-2.980706600495683</v>
       </c>
     </row>
-    <row r="81" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="81">
       <c r="P81">
         <v>-2.7346699226264972</v>
       </c>
     </row>
-    <row r="82" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="82">
       <c r="P82">
         <v>-1.787977180090818</v>
       </c>
     </row>
-    <row r="83" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="83">
       <c r="P83">
         <v>-0.21047573487336371</v>
       </c>
     </row>
-    <row r="84" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="84">
       <c r="P84">
         <v>-2.421424785490963</v>
       </c>
     </row>
-    <row r="85" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="85">
       <c r="P85">
         <v>-1.290839217674141</v>
       </c>
     </row>
-    <row r="86" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="86">
       <c r="P86">
         <v>-1.295696019103886</v>
       </c>
     </row>
-    <row r="87" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="87">
       <c r="P87">
         <v>-1.4106869147492711</v>
       </c>
     </row>
-    <row r="88" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="88">
       <c r="P88">
         <v>-1.19339284630508</v>
       </c>
     </row>
-    <row r="89" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="89">
       <c r="P89">
         <v>-3.536351812235083</v>
       </c>
     </row>
-    <row r="90" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="90">
       <c r="P90">
         <v>-0.60525277755379936</v>
       </c>
     </row>
-    <row r="91" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="91">
       <c r="P91">
         <v>-1.8847307810797029</v>
       </c>
     </row>
-    <row r="92" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="92">
       <c r="P92">
         <v>-1.6438555594496169</v>
       </c>
     </row>
-    <row r="93" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="93">
       <c r="P93">
         <v>-1.299125838736328</v>
       </c>
     </row>
-    <row r="94" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="94">
       <c r="P94">
         <v>-1.5912050777684319</v>
       </c>
     </row>
-    <row r="95" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="95">
       <c r="P95">
         <v>-1.988263565921065</v>
       </c>
     </row>
-    <row r="96" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="96">
       <c r="P96">
         <v>-1.734725021807517</v>
       </c>
     </row>
-    <row r="97" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="97">
       <c r="P97">
         <v>-1.4350096677700761</v>
       </c>
     </row>
-    <row r="98" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="98">
       <c r="P98">
         <v>-1.3848334371730711</v>
       </c>
     </row>
-    <row r="99" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="99">
       <c r="P99">
         <v>-2.4834069271392369</v>
       </c>
     </row>
-    <row r="100" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="100">
       <c r="P100">
         <v>-1.1681071183643059</v>
       </c>
     </row>
-    <row r="101" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="101">
       <c r="P101">
         <v>-2.058798986549677</v>
       </c>
     </row>
-    <row r="102" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="102">
       <c r="P102">
         <v>-1.0010034781517949</v>
       </c>
     </row>
-    <row r="103" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="103">
       <c r="P103">
         <v>-1.8421255194059341</v>
       </c>
     </row>
-    <row r="104" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="104">
       <c r="P104">
         <v>-3.431334841502319</v>
       </c>
     </row>
-    <row r="105" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="105">
       <c r="P105">
         <v>-1.0098983370056209</v>
       </c>
     </row>
-    <row r="106" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="106">
       <c r="P106">
         <v>-0.89872972560697639</v>
       </c>
     </row>
-    <row r="107" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="107">
       <c r="P107">
         <v>-0.87166377948099827</v>
       </c>
     </row>
-    <row r="108" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="108">
       <c r="P108">
         <v>-1.5705377937569669</v>
       </c>
     </row>
-    <row r="109" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="109">
       <c r="P109">
         <v>-0.75910909666968163</v>
       </c>
     </row>
-    <row r="110" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="110">
       <c r="P110">
         <v>-3.2276925566990671</v>
       </c>
     </row>
-    <row r="111" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="111">
       <c r="P111">
         <v>-2.1798955310896422</v>
       </c>
     </row>
-    <row r="112" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="112">
       <c r="P112">
         <v>-3.756718023821862</v>
       </c>
     </row>
-    <row r="113" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="113">
       <c r="P113">
         <v>-1.6436163917782189</v>
       </c>
     </row>
-    <row r="114" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="114">
       <c r="P114">
         <v>-0.94521524551116409</v>
       </c>
     </row>
-    <row r="115" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="115">
       <c r="P115">
         <v>-1.474447686237752</v>
       </c>
     </row>
-    <row r="116" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="116">
       <c r="P116">
         <v>-2.0284827449653768</v>
       </c>
     </row>
-    <row r="117" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="117">
       <c r="P117">
         <v>-1.773511764264236</v>
       </c>
     </row>
-    <row r="118" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="118">
       <c r="P118">
         <v>-1.6090917720035269</v>
       </c>
     </row>
-    <row r="119" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="119">
       <c r="P119">
         <v>-2.397115970960026</v>
       </c>
     </row>
-    <row r="120" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="120">
       <c r="P120">
         <v>-2.1933981714512019</v>
       </c>
     </row>
-    <row r="121" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="121">
       <c r="P121">
         <v>-2.3667475779760458</v>
       </c>
     </row>
-    <row r="122" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="122">
       <c r="P122">
         <v>-1.7875899811302249</v>
       </c>
     </row>
-    <row r="123" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="123">
       <c r="P123">
         <v>-2.88720117976208</v>
       </c>
     </row>
-    <row r="124" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="124">
       <c r="P124">
         <v>0.94272377531366192</v>
       </c>
     </row>
-    <row r="125" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="125">
       <c r="P125">
         <v>-1.770949268369304</v>
       </c>
     </row>
-    <row r="126" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="126">
       <c r="P126">
         <v>-2.8204712468067248</v>
       </c>
     </row>
-    <row r="127" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="127">
       <c r="P127">
         <v>-2.273844373824736</v>
       </c>
     </row>
-    <row r="128" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="128">
       <c r="P128">
         <v>-3.2011661031991352</v>
       </c>
     </row>
-    <row r="129" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="129">
       <c r="P129">
         <v>-1.361350792716177</v>
       </c>
     </row>
-    <row r="130" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="130">
       <c r="P130">
         <v>-1.727700300524019</v>
       </c>
     </row>
-    <row r="131" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="131">
       <c r="P131">
         <v>-2.508296332780569</v>
       </c>
     </row>
-    <row r="132" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="132">
       <c r="P132">
         <v>-2.191950719234216</v>
       </c>
     </row>
-    <row r="133" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="133">
       <c r="P133">
         <v>-1.428969369822449</v>
       </c>
     </row>
-    <row r="134" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="134">
       <c r="P134">
         <v>-1.823566114247317</v>
       </c>
     </row>
-    <row r="135" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="135">
       <c r="P135">
         <v>-1.111605194043902</v>
       </c>
     </row>
-    <row r="136" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="136">
       <c r="P136">
         <v>-1.164963784893178</v>
       </c>
     </row>
-    <row r="137" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="137">
       <c r="P137">
         <v>-2.0885469843464</v>
       </c>
     </row>
-    <row r="138" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="138">
       <c r="P138">
         <v>-2.985918646555791</v>
       </c>
     </row>
-    <row r="139" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="139">
       <c r="P139">
         <v>-2.044858604829229</v>
       </c>
     </row>
-    <row r="140" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="140">
       <c r="P140">
         <v>-2.3788974755538601</v>
       </c>
     </row>
-    <row r="141" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="141">
       <c r="P141">
         <v>-2.0767818220955361</v>
       </c>
     </row>
-    <row r="142" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="142">
       <c r="P142">
         <v>-0.25731526774396762</v>
       </c>
     </row>
-    <row r="143" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="143">
       <c r="P143">
         <v>-1.8856882686170719</v>
       </c>
     </row>
-    <row r="144" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="144">
       <c r="P144">
         <v>-0.25755682975913191</v>
       </c>
     </row>
-    <row r="145" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="145">
       <c r="P145">
         <v>-0.99969581985474154</v>
       </c>
     </row>
-    <row r="146" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="146">
       <c r="P146">
         <v>-5.7198871555739652</v>
       </c>
     </row>
-    <row r="147" spans="16:16" x14ac:dyDescent="0.2">
+    <row r="147">
       <c r="P147">
         <v>-2.1424832467398889</v>
       </c>

</xml_diff>